<commit_message>
fix: enchant cost change & enchants cfg & remove 44
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/EnchantCost_附魔花费表.xlsx
+++ b/pet-simulator/Excel/EnchantCost_附魔花费表.xlsx
@@ -1010,8 +1010,8 @@
   <sheetPr/>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1075,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>5000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1086,7 +1086,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>5000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1097,7 +1097,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1">
-        <v>6000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1108,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="1">
-        <v>7000</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1119,7 +1119,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="1">
-        <v>8000</v>
+        <v>29000</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1130,7 +1130,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="1">
-        <v>10000</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1141,7 +1141,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="1">
-        <v>12000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1152,7 +1152,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="1">
-        <v>14000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1163,7 +1163,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="1">
-        <v>16000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1174,7 +1174,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="1">
-        <v>20000</v>
+        <v>72000</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1185,7 +1185,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="1">
-        <v>20000</v>
+        <v>72000</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>

</xml_diff>